<commit_message>
update test cases for login and acc management
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 3/Iteration 3 Test Cases.xlsx
+++ b/Test Cases/Iteration 3/Iteration 3 Test Cases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smu/Desktop/Ulink/Test Cases/Iteration 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="460" windowWidth="17120" windowHeight="15540" tabRatio="674" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="17300" yWindow="460" windowWidth="17120" windowHeight="15540" tabRatio="674" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis - Doctor" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Client -  CRUD" sheetId="17" state="hidden" r:id="rId7"/>
     <sheet name="Screening - CRUD " sheetId="18" r:id="rId8"/>
     <sheet name="Client - CRUD" sheetId="20" r:id="rId9"/>
-    <sheet name="Login &amp; Create Account" sheetId="21" r:id="rId10"/>
+    <sheet name="Login &amp; Account Management" sheetId="21" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="94">
   <si>
     <t>No</t>
   </si>
@@ -507,14 +507,6 @@
 non-indonesian count = 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Email: 
-Password: 
-Department: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Created </t>
-  </si>
-  <si>
     <t>Login Page Redirect To  Home Page</t>
   </si>
   <si>
@@ -522,13 +514,6 @@
   </si>
   <si>
     <t>Successfully Login - Super Admin  (correct credentials)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail Login </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email: 
-Password: </t>
   </si>
   <si>
     <t>Error Message Shown (Wrong Credentials)</t>
@@ -544,39 +529,92 @@
 Password: xxx</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Account for Medical Team Leader </t>
+    <t xml:space="preserve">Log out </t>
+  </si>
+  <si>
+    <t>Home Page Redirect to Login Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete User Account </t>
+  </si>
+  <si>
+    <t>Create Account - User Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed Login - Input User Account's Old Password </t>
+  </si>
+  <si>
+    <t>Successfully Login - User Account (Test this test case if Test Case 8 pass)</t>
   </si>
   <si>
     <t>Email: ulinkassist_executive@hotmail.com 
-Password:  xxxxxxxx</t>
+Password:  password!23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail Login with non-existence account  </t>
+  </si>
+  <si>
+    <t>Email: admin@ulinkassist.com 
+Password:  p@ssw0rd</t>
+  </si>
+  <si>
+    <t>Email: admin@ulinkassist.com 
+Password:  p@ssw0rd1</t>
+  </si>
+  <si>
+    <t>Login with Test Case 6
+Email: ulinkassist_executive@hotmail.com 
+Password:  password!23
+Click on the logout button</t>
+  </si>
+  <si>
+    <t>Super Admin Change User's Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login with Test Case 6
+Email: ulinkassist_executive@hotmail.com 
+Password:  password!23
+</t>
   </si>
   <si>
     <t xml:space="preserve">Email: ulinkassist_executive@hotmail.com 
-Password:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log out </t>
-  </si>
-  <si>
-    <t>Home Page Redirect to Login Page</t>
-  </si>
-  <si>
-    <t>Login with Test Case 6
-Email: 
-Password: 
-Click on the logout button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete User Account </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login with Test Case 2 
-Email: 
-Password: 
-Select Medical Account (Created in Test Case 4) and Delete </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical Account Removed </t>
+Password:  password123
+</t>
+  </si>
+  <si>
+    <t>Login with Test Case 3
+Email: admin@ulinkassist.com 
+Password:  p@ssw0rd1
+Select User Account (Created in Test Case 4) 
+Email: ulinkassist_executive@hotmail.com , change esisting password to : password123   
+Click Update button</t>
+  </si>
+  <si>
+    <t>Login with Test Case 3
+Email: admin@ulinkassist.com 
+Password:  p@ssw0rd1
+Select User Account (Created in Test Case 4) 
+ulinkassist_executive@hotmail.com 
+and click Delete button and click yes to confirm deletion</t>
+  </si>
+  <si>
+    <t>"Account successfully deleted." shown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Password updated successfully." shown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: ulinkassist_executive@hotmail.com 
+Password:  password
+</t>
+  </si>
+  <si>
+    <t>Email: ulinkassist_executive@hotmail.com 
+Password:  password!23
+Click Create New Account button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Account successfully created" shown </t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,13 +1165,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -1143,13 +1181,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1159,13 +1197,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1178,13 +1216,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1197,13 +1235,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1216,13 +1254,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1235,13 +1273,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1249,18 +1287,18 @@
       <c r="H8" s="2"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1268,30 +1306,57 @@
       <c r="H9" s="2"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+    <row r="10" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+    <row r="11" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+    <row r="12" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -3243,8 +3308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>